<commit_message>
[Test] Load Byte Offset Functions
- Protocol 이 존재할 경우, 그리고 Map Sheet 에 기입이 되어 있을 경우, Byte Offset 과 Protocol Size 를 출력한다.
  (Map Sheet 에 공란 발생시 예외처리를 해줘야하나... 일단 고)
</commit_message>
<xml_diff>
--- a/JRL_Simulator/Win32/Debug/Config/Config_Simulator.xlsx
+++ b/JRL_Simulator/Win32/Debug/Config/Config_Simulator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\03. Rotem\2021. 11. Singapore_JRL\011_Simulator\010_Source\JRL_Simulator\Win32\Debug\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE610007-0EDA-49EF-9C71-7E286F5543E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D540619-8DB4-4D2B-A8CF-04976841ED68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="791" activeTab="1" xr2:uid="{78B8D3DC-9A5B-4C98-B74C-04A1A542662F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="791" activeTab="1" xr2:uid="{78B8D3DC-9A5B-4C98-B74C-04A1A542662F}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="2" r:id="rId1"/>
@@ -1350,7 +1350,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1575,6 +1575,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1904,20 +1907,49 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90D7D11C-CEBF-4B3C-9ACA-7C7791C0172D}">
-  <dimension ref="B2:H39"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.625" customWidth="1"/>
+    <col min="1" max="1" width="2.625" style="75" customWidth="1"/>
     <col min="2" max="5" width="7.625" style="1" customWidth="1"/>
     <col min="6" max="8" width="24.625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="75" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="75">
+        <v>0</v>
+      </c>
+      <c r="B1" s="31">
+        <v>1</v>
+      </c>
+      <c r="C1" s="31">
+        <v>2</v>
+      </c>
+      <c r="D1" s="31">
+        <v>3</v>
+      </c>
+      <c r="E1" s="31">
+        <v>4</v>
+      </c>
+      <c r="F1" s="31">
+        <v>5</v>
+      </c>
+      <c r="G1" s="31">
+        <v>6</v>
+      </c>
+      <c r="H1" s="31">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="75">
+        <v>1</v>
+      </c>
       <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1940,7 +1972,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="75">
+        <v>2</v>
+      </c>
       <c r="B3" s="74" t="s">
         <v>202</v>
       </c>
@@ -1954,7 +1989,10 @@
       <c r="G3" s="73"/>
       <c r="H3" s="73"/>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="75">
+        <v>3</v>
+      </c>
       <c r="B4" s="2">
         <v>0</v>
       </c>
@@ -1975,7 +2013,7 @@
       </c>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B5" s="2">
         <f>+B4+C4</f>
         <v>192</v>
@@ -1997,7 +2035,7 @@
       </c>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B6" s="2">
         <f t="shared" ref="B6:B39" si="0">+B5+C5</f>
         <v>384</v>
@@ -2019,7 +2057,7 @@
       </c>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B7" s="2">
         <f t="shared" si="0"/>
         <v>576</v>
@@ -2041,7 +2079,7 @@
       </c>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B8" s="2">
         <f t="shared" si="0"/>
         <v>768</v>
@@ -2063,7 +2101,7 @@
       </c>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B9" s="2">
         <f t="shared" si="0"/>
         <v>960</v>
@@ -2078,14 +2116,14 @@
         <v>165</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>213</v>
+        <v>191</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>186</v>
       </c>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B10" s="2">
         <f t="shared" si="0"/>
         <v>1152</v>
@@ -2107,7 +2145,7 @@
       </c>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B11" s="2">
         <f t="shared" si="0"/>
         <v>1172</v>
@@ -2129,7 +2167,7 @@
       </c>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B12" s="2">
         <f t="shared" si="0"/>
         <v>1192</v>
@@ -2151,7 +2189,7 @@
       </c>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B13" s="2">
         <f t="shared" si="0"/>
         <v>1212</v>
@@ -2173,7 +2211,7 @@
       </c>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B14" s="2">
         <f t="shared" si="0"/>
         <v>1232</v>
@@ -2195,7 +2233,7 @@
       </c>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B15" s="2">
         <f t="shared" si="0"/>
         <v>1252</v>
@@ -2217,7 +2255,7 @@
       </c>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B16" s="2">
         <f t="shared" si="0"/>
         <v>1272</v>

</xml_diff>